<commit_message>
worldcare row rates update
</commit_message>
<xml_diff>
--- a/Input/Now_Health_Worldcare_ROW/benefits.xlsx
+++ b/Input/Now_Health_Worldcare_ROW/benefits.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="124">
   <si>
     <t xml:space="preserve">PlanName</t>
   </si>
@@ -194,7 +194,23 @@
     <t xml:space="preserve">USD 3,000,000</t>
   </si>
   <si>
-    <t xml:space="preserve">Worldwide excluding USA</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Worldwide excluding USA/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Worldwide including USA</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">In-house network</t>
@@ -278,6 +294,9 @@
     <t xml:space="preserve">10% co-pay</t>
   </si>
   <si>
+    <t xml:space="preserve">Worldwide excluding USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">single</t>
   </si>
   <si>
@@ -305,9 +324,15 @@
     <t xml:space="preserve">IP Psychiatric Treatment- Covered in fulll, limited to 30 days OP Psychiatric Treatment- Covered up to USD 2,500 with $ co-pay/ excess</t>
   </si>
   <si>
+    <t xml:space="preserve">USD 1,000</t>
+  </si>
+  <si>
     <t xml:space="preserve">20% co-pay</t>
   </si>
   <si>
+    <t xml:space="preserve">Worldwide including USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">OP</t>
   </si>
   <si>
@@ -341,6 +366,9 @@
     <t xml:space="preserve">IP Psychiatric Treatment- Covered in fulll, limited to 30 days OP Psychiatric Treatment- Covered up to USD 5,000 $ co-pay/ excess</t>
   </si>
   <si>
+    <t xml:space="preserve">USD 2,500</t>
+  </si>
+  <si>
     <t xml:space="preserve">USD 25 excess</t>
   </si>
   <si>
@@ -368,10 +396,19 @@
     <t xml:space="preserve">IP Psychiatric Treatment- Covered in fulll, limited to 30 days OP Psychiatric Treatment- Covered up to USD 7,500 $ co-pay/ excess</t>
   </si>
   <si>
+    <t xml:space="preserve">USD 5,000</t>
+  </si>
+  <si>
     <t xml:space="preserve">USD 15 excess</t>
   </si>
   <si>
     <t xml:space="preserve">op-option-4/USD 15 excess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD 10,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD 15,000</t>
   </si>
   <si>
     <t xml:space="preserve">addon</t>
@@ -482,7 +519,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,6 +550,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -602,8 +643,8 @@
   </sheetPr>
   <dimension ref="A1:BZ8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BR1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BW4" activeCellId="0" sqref="BW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -970,24 +1011,24 @@
         <v>83</v>
       </c>
       <c r="BW2" s="7" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="BX2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="BY2" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="BZ2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>57</v>
@@ -1027,17 +1068,17 @@
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
@@ -1046,12 +1087,12 @@
       </c>
       <c r="AB3" s="3"/>
       <c r="AC3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
       <c r="AF3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
@@ -1087,11 +1128,11 @@
       </c>
       <c r="AW3" s="3"/>
       <c r="AX3" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BA3" s="3"/>
       <c r="BB3" s="3"/>
@@ -1121,22 +1162,28 @@
       <c r="BR3" s="5"/>
       <c r="BS3" s="4"/>
       <c r="BT3" s="4"/>
+      <c r="BU3" s="0" t="s">
+        <v>94</v>
+      </c>
       <c r="BV3" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="BW3" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="BY3" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="BZ3" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>57</v>
@@ -1176,17 +1223,17 @@
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
@@ -1195,12 +1242,12 @@
       </c>
       <c r="AB4" s="3"/>
       <c r="AC4" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
@@ -1210,23 +1257,23 @@
       </c>
       <c r="AK4" s="3"/>
       <c r="AL4" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="AM4" s="2" t="s">
         <v>72</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AO4" s="3"/>
       <c r="AP4" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AS4" s="3"/>
       <c r="AT4" s="2" t="s">
@@ -1238,11 +1285,11 @@
       </c>
       <c r="AW4" s="3"/>
       <c r="AX4" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="BA4" s="3"/>
       <c r="BB4" s="3"/>
@@ -1272,20 +1319,23 @@
       <c r="BR4" s="5"/>
       <c r="BS4" s="4"/>
       <c r="BT4" s="4"/>
+      <c r="BU4" s="8" t="s">
+        <v>108</v>
+      </c>
       <c r="BV4" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="BW4" s="7"/>
       <c r="BZ4" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>57</v>
@@ -1325,17 +1375,17 @@
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
@@ -1344,38 +1394,38 @@
       </c>
       <c r="AB5" s="3"/>
       <c r="AC5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
       <c r="AF5" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="AK5" s="3"/>
       <c r="AL5" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="AM5" s="2" t="s">
         <v>72</v>
       </c>
       <c r="AN5" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AO5" s="3"/>
       <c r="AP5" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AS5" s="3"/>
       <c r="AT5" s="2" t="s">
@@ -1387,11 +1437,11 @@
       </c>
       <c r="AW5" s="3"/>
       <c r="AX5" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AY5" s="3"/>
       <c r="AZ5" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="BA5" s="3"/>
       <c r="BB5" s="3"/>
@@ -1421,13 +1471,15 @@
       <c r="BR5" s="5"/>
       <c r="BS5" s="4"/>
       <c r="BT5" s="4"/>
-      <c r="BU5" s="4"/>
+      <c r="BU5" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="BV5" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="BW5" s="4"/>
       <c r="BZ5" s="4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,13 +1487,17 @@
       <c r="BR6" s="5"/>
       <c r="BS6" s="4"/>
       <c r="BT6" s="4"/>
-      <c r="BU6" s="4"/>
+      <c r="BU6" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="BV6" s="4"/>
       <c r="BW6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BR7" s="1"/>
-      <c r="BU7" s="4"/>
+      <c r="BU7" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="BV7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1532,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,7 +1561,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1525,7 +1581,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>